<commit_message>
jquery reference changed to https, excel file updated
</commit_message>
<xml_diff>
--- a/Excel_upload.xlsx
+++ b/Excel_upload.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\campaign1\wp-content\plugins\spider-event-calendar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\wordpress\wp-content\plugins\spider-event-calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Tactic upload.xls" sheetId="1" r:id="rId1"/>
-    <sheet name="Channels" sheetId="2" r:id="rId2"/>
+    <sheet name="Channels for Reference" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -921,11 +921,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,35 +1402,26 @@
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
     </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C58" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>Channels!$A$1:$A$75</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C57</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed excel file for channel col
</commit_message>
<xml_diff>
--- a/Excel_upload.xlsx
+++ b/Excel_upload.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\wordpress\wp-content\plugins\spider-event-calendar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selwynax\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Tactic upload.xls" sheetId="1" r:id="rId1"/>
@@ -922,17 +922,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="48.7109375" customWidth="1"/>
   </cols>
@@ -1401,9 +1400,6 @@
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C58" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
latest fixes by Veena
</commit_message>
<xml_diff>
--- a/Excel_upload.xlsx
+++ b/Excel_upload.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selwynax\Desktop\PRAVEENHYD\FromSangeetha\WP_Marcomm_Calendar_V2\spider-event-calendar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praveenkumar.m18\Desktop\Marcom_April\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tactic upload" sheetId="1" r:id="rId1"/>
@@ -42,54 +42,18 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Circuit HR Pages</t>
-  </si>
-  <si>
-    <t>Circuit News</t>
-  </si>
-  <si>
-    <t>Circuit Microsite</t>
-  </si>
-  <si>
-    <t>Wordpress Microsite</t>
-  </si>
-  <si>
-    <t>Ask Vote Answer</t>
-  </si>
-  <si>
-    <t>Double Dutch</t>
-  </si>
-  <si>
-    <t>Physical Poster</t>
-  </si>
-  <si>
-    <t>Digital Sign</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>InsideBlue</t>
-  </si>
-  <si>
     <t>MeetUp</t>
   </si>
   <si>
-    <t>My Intel App</t>
-  </si>
-  <si>
-    <t>Intel Newsroom</t>
-  </si>
-  <si>
     <t>SharePoint</t>
   </si>
   <si>
     <t>Webcast</t>
   </si>
   <si>
-    <t>Enterprise Wiki</t>
-  </si>
-  <si>
     <t>Twitter</t>
   </si>
   <si>
@@ -100,12 +64,48 @@
   </si>
   <si>
     <t>Instagram</t>
+  </si>
+  <si>
+    <t>Circuit_HR_Pages</t>
+  </si>
+  <si>
+    <t>Circuit_News</t>
+  </si>
+  <si>
+    <t>Circuit_Microsite</t>
+  </si>
+  <si>
+    <t>Wordpress_Microsite</t>
+  </si>
+  <si>
+    <t>Ask_Vote_Answer</t>
+  </si>
+  <si>
+    <t>Double_Dutch</t>
+  </si>
+  <si>
+    <t>Physical_Poster</t>
+  </si>
+  <si>
+    <t>Digital_Sign</t>
+  </si>
+  <si>
+    <t>Inside_Blue</t>
+  </si>
+  <si>
+    <t>My_Intel_App</t>
+  </si>
+  <si>
+    <t>Intel_Newsroom</t>
+  </si>
+  <si>
+    <t>Enterprise_Wiki</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,9 +162,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +445,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -475,16 +478,24 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -493,102 +504,102 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
latest excel file from Veena
</commit_message>
<xml_diff>
--- a/Excel_upload.xlsx
+++ b/Excel_upload.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\praveenkumar.m18\Desktop\Marcom_April\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veenaadx\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Tactic upload" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -162,10 +162,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,17 +446,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="50.140625" customWidth="1"/>
@@ -465,7 +466,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -478,19 +479,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>